<commit_message>
Added mechanical and assembly guide.
</commit_message>
<xml_diff>
--- a/src/BOM/SAV MAKER I Rev A - BOM.xlsx
+++ b/src/BOM/SAV MAKER I Rev A - BOM.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="savmakerIBOM.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:fmalpartida:Documents:development:mercurial repos:HW:SAV MAKER I:savmakerIBOM.csv" decimal="," thousands="." comma="1" semicolon="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:fmalpartida:Documents:development:mercurial repos:HW:SAV MAKER I:savmakerIBOM.csv" decimal="," thousands="." comma="1" semicolon="1">
       <textFields count="11">
         <textField/>
         <textField/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="104">
   <si>
     <t>Qty</t>
   </si>
@@ -185,9 +185,6 @@
   </si>
   <si>
     <t>ATMEGA32U4-AU</t>
-  </si>
-  <si>
-    <t>ADAFRUIT_ATMEGA32U4-AU</t>
   </si>
   <si>
     <t>ADAFRUIT_TQFP44</t>
@@ -421,8 +418,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -431,9 +430,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -769,18 +770,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="A1:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="4" width="47.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -804,13 +805,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -872,7 +873,7 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4">
         <v>0.23</v>
@@ -902,7 +903,7 @@
         <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H5">
         <v>2.8000000000000001E-2</v>
@@ -932,7 +933,7 @@
         <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H6">
         <v>2.9000000000000001E-2</v>
@@ -962,7 +963,7 @@
         <v>31</v>
       </c>
       <c r="G7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H7">
         <v>0.1</v>
@@ -992,7 +993,7 @@
         <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H8">
         <v>0.28999999999999998</v>
@@ -1022,7 +1023,7 @@
         <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H9">
         <v>8.9999999999999993E-3</v>
@@ -1052,7 +1053,7 @@
         <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H10">
         <v>3.3000000000000002E-2</v>
@@ -1067,7 +1068,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
         <v>41</v>
@@ -1082,7 +1083,7 @@
         <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H11">
         <v>1.9E-2</v>
@@ -1112,7 +1113,7 @@
         <v>26</v>
       </c>
       <c r="G12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H12">
         <v>1.2E-2</v>
@@ -1142,7 +1143,7 @@
         <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H13">
         <v>0.03</v>
@@ -1160,16 +1161,16 @@
         <v>46</v>
       </c>
       <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
         <v>49</v>
-      </c>
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" t="s">
-        <v>50</v>
       </c>
       <c r="G14" t="s">
         <v>46</v>
@@ -1187,19 +1188,19 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
         <v>51</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F15" t="s">
         <v>53</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" t="s">
-        <v>54</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
@@ -1211,22 +1212,22 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
         <v>85</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
         <v>56</v>
       </c>
-      <c r="D16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" t="s">
-        <v>57</v>
-      </c>
       <c r="G16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H16">
         <v>0.54</v>
@@ -1241,22 +1242,22 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
         <v>58</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
         <v>61</v>
       </c>
-      <c r="D17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" t="s">
-        <v>62</v>
-      </c>
       <c r="G17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H17">
         <v>5.7000000000000002E-2</v>
@@ -1271,16 +1272,16 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
         <v>63</v>
       </c>
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>64</v>
-      </c>
-      <c r="E18" t="s">
-        <v>65</v>
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
@@ -1292,22 +1293,22 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
         <v>67</v>
       </c>
-      <c r="C19" t="s">
+      <c r="F19" t="s">
         <v>69</v>
       </c>
-      <c r="D19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" t="s">
-        <v>70</v>
-      </c>
       <c r="G19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H19">
         <v>0.2</v>
@@ -1322,22 +1323,22 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" t="s">
         <v>71</v>
       </c>
-      <c r="C20" t="s">
+      <c r="F20" t="s">
         <v>73</v>
       </c>
-      <c r="D20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" t="s">
-        <v>74</v>
-      </c>
       <c r="G20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H20">
         <v>0.27400000000000002</v>
@@ -1352,22 +1353,22 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" t="s">
         <v>75</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" t="s">
         <v>78</v>
       </c>
-      <c r="D21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" t="s">
-        <v>77</v>
-      </c>
-      <c r="F21" t="s">
-        <v>79</v>
-      </c>
       <c r="G21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H21">
         <v>0.09</v>
@@ -1382,16 +1383,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" t="s">
         <v>80</v>
       </c>
-      <c r="C22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>81</v>
-      </c>
-      <c r="E22" t="s">
-        <v>82</v>
       </c>
       <c r="H22">
         <v>4.5</v>
@@ -1403,7 +1404,7 @@
     </row>
     <row r="26" spans="1:9" ht="18">
       <c r="H26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I26" s="1">
         <f>SUM(I2:I22)</f>

</xml_diff>